<commit_message>
김다희 MiningNumMin MiningNumMax 추가
</commit_message>
<xml_diff>
--- a/Design/DataTable/GlobalSystem.xlsx
+++ b/Design/DataTable/GlobalSystem.xlsx
@@ -5,27 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ComputerScience\Project\PlumTowerDefence\PlumTowerDefecne\Design\DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdhhi\Desktop\서울과학기술대학교\PLUM\2022 8월 게임 프로젝트\PlumTowerDefecne\Design\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44631C1-8ADF-48D2-B24D-33D3EA02EDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61A5C61-FC50-4C27-91E5-5304C34F9D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,6 +67,22 @@
   </si>
   <si>
     <t>증강체 버프  개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MiningNumMin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MiningNumMax</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>채굴최소횟수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>채굴최대횟수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -63,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +102,13 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -99,10 +133,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -384,24 +421,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D20" sqref="D20:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="18.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.09765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="64.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="8.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.8984375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,7 +452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -429,7 +466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -441,6 +478,34 @@
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>